<commit_message>
Regenerate test data to include credit card account refund/credit transactions.
</commit_message>
<xml_diff>
--- a/tests/test_xls/sheet_accounts/test_basic/expected_result.xlsx
+++ b/tests/test_xls/sheet_accounts/test_basic/expected_result.xlsx
@@ -533,7 +533,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" s="2" t="n">
-        <v>43101</v>
+        <v>43104</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>44926</v>
@@ -565,7 +565,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" s="2" t="n">
-        <v>43102</v>
+        <v>43101</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>44926</v>
@@ -597,7 +597,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" s="2" t="n">
-        <v>43103</v>
+        <v>43101</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>44926</v>
@@ -629,7 +629,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" s="2" t="n">
-        <v>43101</v>
+        <v>43102</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>44926</v>

</xml_diff>